<commit_message>
create hmw 3 Postman task 1
</commit_message>
<xml_diff>
--- a/hmw_3_Postman_Strashchenko.xlsx
+++ b/hmw_3_Postman_Strashchenko.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>1.8</t>
+  </si>
+  <si>
+    <t>1,23</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:D17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,8 +637,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>1.23</v>
+      <c r="A10" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
update hmw 3 xlsx
</commit_message>
<xml_diff>
--- a/hmw_3_Postman_Strashchenko.xlsx
+++ b/hmw_3_Postman_Strashchenko.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -110,13 +110,7 @@
     <t>17</t>
   </si>
   <si>
-    <t>1,8</t>
-  </si>
-  <si>
     <t>1.8</t>
-  </si>
-  <si>
-    <t>1,23</t>
   </si>
 </sst>
 </file>
@@ -495,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +536,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="3">
-        <f t="shared" ref="B3:B14" si="0">LEN(A3)</f>
+        <f t="shared" ref="B3:B15" si="0">LEN(A3)</f>
         <v>3</v>
       </c>
       <c r="C3" s="2">
@@ -638,7 +632,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <f t="shared" si="0"/>
@@ -653,7 +647,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3">
         <f t="shared" si="0"/>
@@ -668,11 +662,11 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>10</v>
@@ -682,12 +676,12 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
+      <c r="A13" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B13" s="3">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
@@ -697,12 +691,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="B14" s="3">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>28</v>
@@ -713,39 +705,32 @@
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="10"/>
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update hmw 3 Postman task 1
</commit_message>
<xml_diff>
--- a/hmw_3_Postman_Strashchenko.xlsx
+++ b/hmw_3_Postman_Strashchenko.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>1.8</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -177,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -190,9 +196,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -492,21 +495,21 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A17" sqref="A17:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="9" customWidth="1"/>
-    <col min="3" max="4" width="38.5703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="8" customWidth="1"/>
+    <col min="3" max="4" width="38.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -710,15 +713,15 @@
         <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="10"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
@@ -726,11 +729,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>